<commit_message>
collect from PONDR checked
</commit_message>
<xml_diff>
--- a/output/table_s1/VL3-BA.xlsx
+++ b/output/table_s1/VL3-BA.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
minor typo and fig2 raw data created
</commit_message>
<xml_diff>
--- a/output/table_s1/VL3-BA.xlsx
+++ b/output/table_s1/VL3-BA.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>&gt;20</t>
+          <t>&gt;=20</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -496,7 +496,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>&gt;30</t>
+          <t>&gt;=30</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -521,7 +521,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>&gt;40</t>
+          <t>&gt;=40</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -546,7 +546,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>&gt;50</t>
+          <t>&gt;=50</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -571,7 +571,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>&gt;60</t>
+          <t>&gt;=60</t>
         </is>
       </c>
       <c r="C6" t="n">

</xml_diff>